<commit_message>
Add bag report Login page. Email field 1
</commit_message>
<xml_diff>
--- a/Choice_Stationery_Supplies_Bug_Reports_Login_page_Email_field.xlsx
+++ b/Choice_Stationery_Supplies_Bug_Reports_Login_page_Email_field.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="155">
   <si>
     <t>Created by</t>
   </si>
@@ -584,27 +584,6 @@
   <si>
     <t>The user 
 email is  started with any symbols</t>
-  </si>
-  <si>
-    <t>BAG_ 04</t>
-  </si>
-  <si>
-    <t>TC_log_14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> The Max length of the "Email" field is not specified</t>
-  </si>
-  <si>
-    <t>1.Open Browser 
-2.Open URL
-3.Go to the Login page
-4.Enter the maximum allowed length value in the "Email" field.</t>
-  </si>
-  <si>
-    <t>The "Email" field does not allow  to enter a value longer than 128 characters</t>
-  </si>
-  <si>
-    <t>The "Email" field  allow  a value longer than 128 characters</t>
   </si>
   <si>
     <r>
@@ -1886,10 +1865,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1945,7 +1924,7 @@
         <v>123</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
@@ -2057,32 +2036,6 @@
         <v>151</v>
       </c>
       <c r="H15" s="32" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="C16" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="F16" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>151</v>
-      </c>
-      <c r="H16" s="32" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>